<commit_message>
juicy small changes to make webapp work
</commit_message>
<xml_diff>
--- a/AI_Stock_Live_Comparison_20250719_100237.xlsx
+++ b/AI_Stock_Live_Comparison_20250719_100237.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -377,16 +377,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -402,1255 +406,1361 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="7.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="7.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>159.205</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>0.25813499904</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>115.365944</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>798940800</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="1" t="n">
         <v>131.9459</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="1" t="n">
         <v>17.51</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="1" t="n">
         <v>7.19</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2" s="1" t="n">
         <v>11.27</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="1" t="n">
         <v>16.63</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="1" t="n">
         <v>170</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>512.72</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>3.810811707392</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>39.653515</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>1755734400</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>0.67</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="1" t="n">
         <v>522.2628</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3" s="1" t="n">
         <v>26.35</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="1" t="n">
         <v>1.99</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="L3" s="1" t="n">
         <v>4.3</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="1" t="n">
         <v>7.27</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="1" t="n">
         <v>545</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>173.6875</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>4.235821318144</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>56.02823</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>1749600000</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <v>0.03</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="1" t="n">
         <v>173.91614</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="1" t="n">
         <v>18.38</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="1" t="n">
         <v>5.49</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="L4" s="1" t="n">
         <v>9.33</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="M4" s="1" t="n">
         <v>14.61</v>
       </c>
-      <c r="N4" s="0" t="n">
+      <c r="N4" s="1" t="n">
         <v>185</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>701.0265</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>1.762611953664</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>27.415976</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>1750032000</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>0.28</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="1" t="n">
         <v>729.36505</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="J5" s="1" t="n">
         <v>55.98</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="K5" s="1" t="n">
         <v>3.99</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="L5" s="1" t="n">
         <v>7.44</v>
       </c>
-      <c r="M5" s="0" t="n">
+      <c r="M5" s="1" t="n">
         <v>11.75</v>
       </c>
-      <c r="N5" s="0" t="n">
+      <c r="N5" s="1" t="n">
         <v>745</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>223.56</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>2.373402230784</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>36.410423</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6" s="1" t="n">
         <v>241.81862</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="J6" s="1" t="n">
         <v>16.24</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6" s="1" t="n">
         <v>3.15</v>
       </c>
-      <c r="L6" s="0" t="n">
+      <c r="L6" s="1" t="n">
         <v>6.11</v>
       </c>
-      <c r="M6" s="0" t="n">
+      <c r="M6" s="1" t="n">
         <v>10.23</v>
       </c>
-      <c r="N6" s="0" t="n">
+      <c r="N6" s="1" t="n">
         <v>240</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>183.85</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>2.225632968704</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>20.496098</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>1749427200</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="1" t="n">
         <v>0.47</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="1" t="n">
         <v>199.625</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="J7" s="1" t="n">
         <v>12.75</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7" s="1" t="n">
         <v>4.03</v>
       </c>
-      <c r="L7" s="0" t="n">
+      <c r="L7" s="1" t="n">
         <v>6.94</v>
       </c>
-      <c r="M7" s="0" t="n">
+      <c r="M7" s="1" t="n">
         <v>10.45</v>
       </c>
-      <c r="N7" s="0" t="n">
+      <c r="N7" s="1" t="n">
         <v>195</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>210.9155</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>3.150191525888</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>32.80179</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>1747008000</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="1" t="n">
         <v>0.51</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I8" s="1" t="n">
         <v>228.60326</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="J8" s="1" t="n">
         <v>12.2</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K8" s="1" t="n">
         <v>2.87</v>
       </c>
-      <c r="L8" s="0" t="n">
+      <c r="L8" s="1" t="n">
         <v>5.38</v>
       </c>
-      <c r="M8" s="0" t="n">
+      <c r="M8" s="1" t="n">
         <v>8.51</v>
       </c>
-      <c r="N8" s="0" t="n">
+      <c r="N8" s="1" t="n">
         <v>225</v>
       </c>
-      <c r="AB8" s="0" t="s">
+      <c r="AB8" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>320.656</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>1.03282016256</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>184.28506</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I9" s="1" t="n">
         <v>306.07172</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="J9" s="1" t="n">
         <v>48.6</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="K9" s="1" t="n">
         <v>8.58</v>
       </c>
-      <c r="L9" s="0" t="n">
+      <c r="L9" s="1" t="n">
         <v>13.88</v>
       </c>
-      <c r="M9" s="0" t="n">
+      <c r="M9" s="1" t="n">
         <v>20.89</v>
       </c>
-      <c r="N9" s="0" t="n">
+      <c r="N9" s="1" t="n">
         <v>340</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>281.715</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>0.261825069056</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>48.15641</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>1746748800</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="1" t="n">
         <v>2.28</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="I10" s="1" t="n">
         <v>258.022</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="J10" s="1" t="n">
         <v>19.75</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="K10" s="1" t="n">
         <v>3.19</v>
       </c>
-      <c r="L10" s="0" t="n">
+      <c r="L10" s="1" t="n">
         <v>5.66</v>
       </c>
-      <c r="M10" s="0" t="n">
+      <c r="M10" s="1" t="n">
         <v>8.25</v>
       </c>
-      <c r="N10" s="0" t="n">
+      <c r="N10" s="1" t="n">
         <v>300</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>247.5212</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>0.695244947456</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>57.16425</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>1752105600</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="1" t="n">
         <v>0.91</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="I11" s="1" t="n">
         <v>215.22266</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="J11" s="1" t="n">
         <v>25.93</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="K11" s="1" t="n">
         <v>5.1</v>
       </c>
-      <c r="L11" s="0" t="n">
+      <c r="L11" s="1" t="n">
         <v>8.67</v>
       </c>
-      <c r="M11" s="0" t="n">
+      <c r="M11" s="1" t="n">
         <v>13.67</v>
       </c>
-      <c r="N11" s="0" t="n">
+      <c r="N11" s="1" t="n">
         <v>270</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>60.885</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>0.010540167168</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="I12" s="1" t="n">
         <v>66.7</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="J12" s="1" t="n">
         <v>13.86</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="K12" s="1" t="n">
         <v>13.14</v>
       </c>
-      <c r="L12" s="0" t="n">
+      <c r="L12" s="1" t="n">
         <v>20.2</v>
       </c>
-      <c r="M12" s="0" t="n">
+      <c r="M12" s="1" t="n">
         <v>27.81</v>
       </c>
-      <c r="N12" s="0" t="n">
+      <c r="N12" s="1" t="n">
         <v>65</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>156.99</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>0.254543609856</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>114.59125</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="G13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="I13" s="1" t="n">
         <v>131.9459</v>
       </c>
-      <c r="J13" s="0" t="n">
+      <c r="J13" s="1" t="n">
         <v>17.55</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="K13" s="1" t="n">
         <v>5.99</v>
       </c>
-      <c r="L13" s="0" t="n">
+      <c r="L13" s="1" t="n">
         <v>10.13</v>
       </c>
-      <c r="M13" s="0" t="n">
+      <c r="M13" s="1" t="n">
         <v>15.62</v>
       </c>
-      <c r="N13" s="0" t="n">
+      <c r="N13" s="1" t="n">
         <v>170</v>
       </c>
-      <c r="P13" s="0" t="s">
+      <c r="P13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q13" s="0" t="n">
+      <c r="Q13" s="1" t="n">
         <v>11.18</v>
       </c>
-      <c r="R13" s="0" t="n">
+      <c r="R13" s="1" t="n">
         <v>9.95</v>
       </c>
-      <c r="S13" s="1" t="n">
+      <c r="S13" s="2" t="n">
         <f aca="false">Q13/R13</f>
         <v>1.12361809045226</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>510.05</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>3.790967144448</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>39.35571</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="G14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14" s="1" t="n">
         <v>0.67</v>
       </c>
-      <c r="I14" s="0" t="n">
+      <c r="I14" s="1" t="n">
         <v>522.2628</v>
       </c>
-      <c r="J14" s="0" t="n">
+      <c r="J14" s="1" t="n">
         <v>25.55</v>
       </c>
-      <c r="K14" s="0" t="n">
+      <c r="K14" s="1" t="n">
         <v>1.69</v>
       </c>
-      <c r="L14" s="0" t="n">
+      <c r="L14" s="1" t="n">
         <v>4.11</v>
       </c>
-      <c r="M14" s="0" t="n">
+      <c r="M14" s="1" t="n">
         <v>7.16</v>
       </c>
-      <c r="N14" s="0" t="n">
+      <c r="N14" s="1" t="n">
         <v>545</v>
       </c>
-      <c r="P14" s="0" t="s">
+      <c r="P14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q14" s="0" t="n">
+      <c r="Q14" s="1" t="n">
         <v>5.01</v>
       </c>
-      <c r="R14" s="0" t="n">
+      <c r="R14" s="1" t="n">
         <v>1.4</v>
       </c>
-      <c r="S14" s="1" t="n">
+      <c r="S14" s="2" t="n">
         <f aca="false">Q14/R14</f>
         <v>3.57857142857143</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>172.41</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>4.204666290176</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>55.61613</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="G15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="1" t="n">
         <v>0.03</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="I15" s="1" t="n">
         <v>173.91614</v>
       </c>
-      <c r="J15" s="0" t="n">
+      <c r="J15" s="1" t="n">
         <v>18.75</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="K15" s="1" t="n">
         <v>4.99</v>
       </c>
-      <c r="L15" s="0" t="n">
+      <c r="L15" s="1" t="n">
         <v>9.34</v>
       </c>
-      <c r="M15" s="0" t="n">
+      <c r="M15" s="1" t="n">
         <v>14.45</v>
       </c>
-      <c r="N15" s="0" t="n">
+      <c r="N15" s="1" t="n">
         <v>183</v>
       </c>
-      <c r="P15" s="0" t="s">
+      <c r="P15" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q15" s="0" t="n">
+      <c r="Q15" s="1" t="n">
         <v>10.88</v>
       </c>
-      <c r="R15" s="0" t="n">
+      <c r="R15" s="1" t="n">
         <v>8.38</v>
       </c>
-      <c r="S15" s="1" t="n">
+      <c r="S15" s="2" t="n">
         <f aca="false">Q15/R15</f>
         <v>1.29832935560859</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>704.28</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>1.7707925504</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>27.543217</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="G16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16" s="1" t="n">
         <v>0.28</v>
       </c>
-      <c r="I16" s="0" t="n">
+      <c r="I16" s="1" t="n">
         <v>729.36505</v>
       </c>
-      <c r="J16" s="0" t="n">
+      <c r="J16" s="1" t="n">
         <v>60.65</v>
       </c>
-      <c r="K16" s="0" t="n">
+      <c r="K16" s="1" t="n">
         <v>3.95</v>
       </c>
-      <c r="L16" s="0" t="n">
+      <c r="L16" s="1" t="n">
         <v>7.15</v>
       </c>
-      <c r="M16" s="0" t="n">
+      <c r="M16" s="1" t="n">
         <v>11.4</v>
       </c>
-      <c r="N16" s="0" t="n">
+      <c r="N16" s="1" t="n">
         <v>750</v>
       </c>
-      <c r="P16" s="0" t="s">
+      <c r="P16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q16" s="0" t="n">
+      <c r="Q16" s="1" t="n">
         <v>8.61</v>
       </c>
-      <c r="R16" s="0" t="n">
+      <c r="R16" s="1" t="n">
         <v>1.62</v>
       </c>
-      <c r="S16" s="1" t="n">
+      <c r="S16" s="2" t="n">
         <f aca="false">Q16/R16</f>
         <v>5.31481481481481</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>226.13</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>2.400686440448</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>36.769108</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="I17" s="1" t="n">
         <v>241.81862</v>
       </c>
-      <c r="J17" s="0" t="n">
+      <c r="J17" s="1" t="n">
         <v>15.42</v>
       </c>
-      <c r="K17" s="0" t="n">
+      <c r="K17" s="1" t="n">
         <v>3.41</v>
       </c>
-      <c r="L17" s="0" t="n">
+      <c r="L17" s="1" t="n">
         <v>6.5</v>
       </c>
-      <c r="M17" s="0" t="n">
+      <c r="M17" s="1" t="n">
         <v>10.53</v>
       </c>
-      <c r="N17" s="0" t="n">
+      <c r="N17" s="1" t="n">
         <v>240</v>
       </c>
-      <c r="P17" s="0" t="s">
+      <c r="P17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q17" s="0" t="n">
+      <c r="Q17" s="1" t="n">
         <v>6.82</v>
       </c>
-      <c r="R17" s="0" t="n">
+      <c r="R17" s="1" t="n">
         <v>4.66</v>
       </c>
-      <c r="S17" s="1" t="n">
+      <c r="S17" s="2" t="n">
         <f aca="false">Q17/R17</f>
         <v>1.46351931330472</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>185.94</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>2.250934059008</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>20.752232</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="G18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H18" s="1" t="n">
         <v>0.47</v>
       </c>
-      <c r="I18" s="0" t="n">
+      <c r="I18" s="1" t="n">
         <v>199.625</v>
       </c>
-      <c r="J18" s="0" t="n">
+      <c r="J18" s="1" t="n">
         <v>11.84</v>
       </c>
-      <c r="K18" s="0" t="n">
+      <c r="K18" s="1" t="n">
         <v>3.35</v>
       </c>
-      <c r="L18" s="0" t="n">
+      <c r="L18" s="1" t="n">
         <v>6.16</v>
       </c>
-      <c r="M18" s="0" t="n">
+      <c r="M18" s="1" t="n">
         <v>9.86</v>
       </c>
-      <c r="N18" s="0" t="n">
+      <c r="N18" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="P18" s="0" t="s">
+      <c r="P18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q18" s="0" t="n">
+      <c r="Q18" s="1" t="n">
         <v>6.37</v>
       </c>
-      <c r="R18" s="0" t="n">
+      <c r="R18" s="1" t="n">
         <v>5.3</v>
       </c>
-      <c r="S18" s="1" t="n">
+      <c r="S18" s="2" t="n">
         <f aca="false">Q18/R18</f>
         <v>1.20188679245283</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>211.18</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>3.154142035968</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>32.89408</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="G19" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="H19" s="1" t="n">
         <v>0.51</v>
       </c>
-      <c r="I19" s="0" t="n">
+      <c r="I19" s="1" t="n">
         <v>228.60326</v>
       </c>
-      <c r="J19" s="0" t="n">
+      <c r="J19" s="1" t="n">
         <v>12.3</v>
       </c>
-      <c r="K19" s="0" t="n">
+      <c r="K19" s="1" t="n">
         <v>2.75</v>
       </c>
-      <c r="L19" s="0" t="n">
+      <c r="L19" s="1" t="n">
         <v>5.23</v>
       </c>
-      <c r="M19" s="0" t="n">
+      <c r="M19" s="1" t="n">
         <v>8.57</v>
       </c>
-      <c r="N19" s="0" t="n">
+      <c r="N19" s="1" t="n">
         <v>225</v>
       </c>
-      <c r="P19" s="0" t="s">
+      <c r="P19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q19" s="0" t="n">
+      <c r="Q19" s="1" t="n">
         <v>5.82</v>
       </c>
-      <c r="R19" s="0" t="n">
+      <c r="R19" s="1" t="n">
         <v>4.06</v>
       </c>
-      <c r="S19" s="1" t="n">
+      <c r="S19" s="2" t="n">
         <f aca="false">Q19/R19</f>
         <v>1.43349753694581</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <v>329.65</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="1" t="n">
         <v>1.061789433856</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>188.37143</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I20" s="0" t="n">
+      <c r="I20" s="1" t="n">
         <v>306.07172</v>
       </c>
-      <c r="J20" s="0" t="n">
+      <c r="J20" s="1" t="n">
         <v>46.7</v>
       </c>
-      <c r="K20" s="0" t="n">
+      <c r="K20" s="1" t="n">
         <v>8.54</v>
       </c>
-      <c r="L20" s="0" t="n">
+      <c r="L20" s="1" t="n">
         <v>13.65</v>
       </c>
-      <c r="M20" s="0" t="n">
+      <c r="M20" s="1" t="n">
         <v>20.26</v>
       </c>
-      <c r="N20" s="0" t="n">
+      <c r="N20" s="1" t="n">
         <v>350</v>
       </c>
-      <c r="P20" s="0" t="s">
+      <c r="P20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q20" s="0" t="n">
+      <c r="Q20" s="1" t="n">
         <v>14.17</v>
       </c>
-      <c r="R20" s="0" t="n">
+      <c r="R20" s="1" t="n">
         <v>6.15</v>
       </c>
-      <c r="S20" s="1" t="n">
+      <c r="S20" s="2" t="n">
         <f aca="false">Q20/R20</f>
         <v>2.30406504065041</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="1" t="n">
         <v>285.87</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="1" t="n">
         <v>0.26568671232</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>48.783276</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G21" s="0" t="s">
+      <c r="G21" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21" s="1" t="n">
         <v>2.28</v>
       </c>
-      <c r="I21" s="0" t="n">
+      <c r="I21" s="1" t="n">
         <v>258.022</v>
       </c>
-      <c r="J21" s="0" t="n">
+      <c r="J21" s="1" t="n">
         <v>18.75</v>
       </c>
-      <c r="K21" s="0" t="n">
+      <c r="K21" s="1" t="n">
         <v>2.99</v>
       </c>
-      <c r="L21" s="0" t="n">
+      <c r="L21" s="1" t="n">
         <v>5.61</v>
       </c>
-      <c r="M21" s="0" t="n">
+      <c r="M21" s="1" t="n">
         <v>7.57</v>
       </c>
-      <c r="N21" s="0" t="n">
+      <c r="N21" s="1" t="n">
         <v>305</v>
       </c>
-      <c r="P21" s="0" t="s">
+      <c r="P21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q21" s="0" t="n">
+      <c r="Q21" s="1" t="n">
         <v>6.56</v>
       </c>
-      <c r="R21" s="0" t="n">
+      <c r="R21" s="1" t="n">
         <v>2.65</v>
       </c>
-      <c r="S21" s="1" t="n">
+      <c r="S21" s="2" t="n">
         <f aca="false">Q21/R21</f>
         <v>2.47547169811321</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="1" t="n">
         <v>245.45</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="1" t="n">
         <v>0.689427316736</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="1" t="n">
         <v>56.555298</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="F22" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G22" s="0" t="s">
+      <c r="G22" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="H22" s="1" t="n">
         <v>0.91</v>
       </c>
-      <c r="I22" s="0" t="n">
+      <c r="I22" s="1" t="n">
         <v>215.22266</v>
       </c>
-      <c r="J22" s="0" t="n">
+      <c r="J22" s="1" t="n">
         <v>25.73</v>
       </c>
-      <c r="K22" s="0" t="n">
+      <c r="K22" s="1" t="n">
         <v>4.73</v>
       </c>
-      <c r="L22" s="0" t="n">
+      <c r="L22" s="1" t="n">
         <v>8.39</v>
       </c>
-      <c r="M22" s="0" t="n">
+      <c r="M22" s="1" t="n">
         <v>12.98</v>
       </c>
-      <c r="N22" s="0" t="n">
+      <c r="N22" s="1" t="n">
         <v>270</v>
       </c>
-      <c r="P22" s="0" t="s">
+      <c r="P22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q22" s="0" t="n">
+      <c r="Q22" s="1" t="n">
         <v>10.48</v>
       </c>
-      <c r="R22" s="0" t="n">
+      <c r="R22" s="1" t="n">
         <v>5.29</v>
       </c>
-      <c r="S22" s="1" t="n">
+      <c r="S22" s="2" t="n">
         <f aca="false">Q22/R22</f>
         <v>1.98109640831758</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="1" t="n">
         <v>60.98</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="1" t="n">
         <v>0.010556613632</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="F23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I23" s="0" t="n">
+      <c r="I23" s="1" t="n">
         <v>66.7</v>
       </c>
-      <c r="J23" s="0" t="n">
+      <c r="J23" s="1" t="n">
         <v>13.5</v>
       </c>
-      <c r="K23" s="0" t="n">
+      <c r="K23" s="1" t="n">
         <v>11.89</v>
       </c>
-      <c r="L23" s="0" t="n">
+      <c r="L23" s="1" t="n">
         <v>18.53</v>
       </c>
-      <c r="M23" s="0" t="n">
+      <c r="M23" s="1" t="n">
         <v>26.24</v>
       </c>
-      <c r="N23" s="0" t="n">
+      <c r="N23" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="P23" s="0" t="s">
+      <c r="P23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q23" s="0" t="n">
+      <c r="Q23" s="1" t="n">
         <v>22.14</v>
       </c>
-      <c r="R23" s="0" t="n">
+      <c r="R23" s="1" t="n">
         <v>43.03</v>
       </c>
-      <c r="S23" s="1" t="n">
+      <c r="S23" s="2" t="n">
         <f aca="false">Q23/R23</f>
         <v>0.514524750174297</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="1" t="n">
         <v>349.05</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="1" t="n">
         <v>0.681869180928</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="1" t="n">
         <v>35.080402</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="F24" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="G24" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24" s="1" t="n">
         <v>0.66</v>
       </c>
-      <c r="I24" s="0" t="n">
+      <c r="I24" s="1" t="n">
         <v>382.39975</v>
       </c>
-      <c r="J24" s="0" t="n">
+      <c r="J24" s="1" t="n">
         <v>17.81</v>
       </c>
-      <c r="K24" s="0" t="n">
+      <c r="K24" s="1" t="n">
         <v>2.21</v>
       </c>
-      <c r="L24" s="0" t="n">
+      <c r="L24" s="1" t="n">
         <v>4.31</v>
       </c>
-      <c r="M24" s="0" t="n">
+      <c r="M24" s="1" t="n">
         <v>7.32</v>
       </c>
-      <c r="N24" s="0" t="n">
+      <c r="N24" s="1" t="n">
         <v>370</v>
       </c>
-      <c r="P24" s="0" t="s">
+      <c r="P24" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q24" s="0" t="n">
+      <c r="Q24" s="1" t="n">
         <v>5.1</v>
       </c>
-      <c r="R24" s="0" t="n">
+      <c r="R24" s="1" t="n">
         <v>2.1</v>
       </c>
-      <c r="S24" s="1" t="n">
+      <c r="S24" s="2" t="n">
         <f aca="false">Q24/R24</f>
         <v>2.42857142857143</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="1" t="n">
         <v>574.6</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="1" t="n">
         <v>0.156828450816</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="1" t="n">
         <v>82.676254</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="F25" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G25" s="0" t="s">
+      <c r="G25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H25" s="1" t="n">
         <v>0.19</v>
       </c>
-      <c r="I25" s="0" t="n">
+      <c r="I25" s="1" t="n">
         <v>454.61963</v>
       </c>
-      <c r="J25" s="0" t="n">
+      <c r="J25" s="1" t="n">
         <v>75.16</v>
       </c>
-      <c r="K25" s="0" t="n">
+      <c r="K25" s="1" t="n">
         <v>6.25</v>
       </c>
-      <c r="L25" s="0" t="n">
+      <c r="L25" s="1" t="n">
         <v>11.05</v>
       </c>
-      <c r="M25" s="0" t="n">
+      <c r="M25" s="1" t="n">
         <v>15.8</v>
       </c>
-      <c r="N25" s="0" t="n">
+      <c r="N25" s="1" t="n">
         <v>610</v>
       </c>
-      <c r="P25" s="0" t="s">
+      <c r="P25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q25" s="0" t="n">
+      <c r="Q25" s="1" t="n">
         <v>13.08</v>
       </c>
-      <c r="R25" s="0" t="n">
+      <c r="R25" s="1" t="n">
         <v>2.75</v>
       </c>
-      <c r="S25" s="1" t="n">
+      <c r="S25" s="2" t="n">
         <f aca="false">Q25/R25</f>
         <v>4.75636363636364</v>
       </c>

</xml_diff>